<commit_message>
updated column headers in excel
</commit_message>
<xml_diff>
--- a/output/Results.xlsx
+++ b/output/Results.xlsx
@@ -20,7 +20,7 @@
     <t>Betting Site</t>
   </si>
   <si>
-    <t>Difference</t>
+    <t>Confidence</t>
   </si>
   <si>
     <t>Payout</t>
@@ -368,7 +368,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="11.69140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.5390625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.92578125" customWidth="true" bestFit="true"/>
   </cols>
@@ -543,7 +543,7 @@
   <cols>
     <col min="1" max="1" width="13.19921875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.69140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.5390625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.92578125" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>